<commit_message>
Excel style has been changed
</commit_message>
<xml_diff>
--- a/src/main/chungus.xlsx
+++ b/src/main/chungus.xlsx
@@ -35,7 +35,7 @@
     <font>
       <name val="Arial"/>
       <sz val="11.0"/>
-      <color indexed="8"/>
+      <color indexed="9"/>
       <b val="true"/>
     </font>
     <font>
@@ -75,12 +75,12 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="DCE6F1"/>
+        <fgColor rgb="012A49"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="DCE6F1"/>
+        <fgColor rgb="012A49"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,8 +120,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFill="true" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment wrapText="true" vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="true" applyAlignment="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyAlignment="true" applyFont="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
@@ -145,6 +149,25 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="21.875" customWidth="true"/>
+    <col min="2" max="2" width="21.875" customWidth="true"/>
+    <col min="3" max="3" width="21.875" customWidth="true"/>
+    <col min="4" max="4" width="21.875" customWidth="true"/>
+    <col min="5" max="5" width="21.875" customWidth="true"/>
+    <col min="6" max="6" width="21.875" customWidth="true"/>
+    <col min="7" max="7" width="21.875" customWidth="true"/>
+    <col min="8" max="8" width="21.875" customWidth="true"/>
+    <col min="9" max="9" width="21.875" customWidth="true"/>
+    <col min="10" max="10" width="21.875" customWidth="true"/>
+    <col min="11" max="11" width="21.875" customWidth="true"/>
+    <col min="12" max="12" width="21.875" customWidth="true"/>
+    <col min="13" max="13" width="21.875" customWidth="true"/>
+    <col min="14" max="14" width="21.875" customWidth="true"/>
+    <col min="15" max="15" width="21.875" customWidth="true"/>
+    <col min="16" max="16" width="21.875" customWidth="true"/>
+    <col min="17" max="17" width="21.875" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="inlineStr">

</xml_diff>